<commit_message>
calorimetry : scripts : data load : correction
</commit_message>
<xml_diff>
--- a/input/calorimetry/ds.3.ampoule/test_3.xlsx
+++ b/input/calorimetry/ds.3.ampoule/test_3.xlsx
@@ -5,15 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="input_k_constants_log10" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="input_concentrations" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="heats" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="targets" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="enthalpies" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="setup" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="heats" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="targets" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="enthalpies" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t xml:space="preserve">H</t>
   </si>
@@ -84,6 +85,18 @@
     <t xml:space="preserve">h</t>
   </si>
   <si>
+    <t xml:space="preserve">Calorimeter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ampoule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">component</t>
+  </si>
+  <si>
     <t xml:space="preserve">data</t>
   </si>
   <si>
@@ -97,9 +110,6 @@
   </si>
   <si>
     <t xml:space="preserve">constants </t>
-  </si>
-  <si>
-    <t xml:space="preserve">component</t>
   </si>
   <si>
     <t xml:space="preserve">Reaction</t>
@@ -645,10 +655,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -660,145 +670,24 @@
       <c r="A1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>8</v>
+      <c r="B1" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>-10.0952</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>-10.4137</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>-10.8359</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>-10.7336</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>-9.776</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>-9.9857</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>-9.7711</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>-9.8545</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>18</v>
+      <c r="B3" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -817,10 +706,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -832,19 +721,145 @@
       <c r="A1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="F1" s="0" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>1</v>
+      <c r="B2" s="0" t="n">
+        <v>-10.0952</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>-10.4137</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>-10.8359</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>-10.7336</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>-9.776</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>-9.9857</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>-9.7711</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>-9.8545</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -859,6 +874,38 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -876,10 +923,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>